<commit_message>
change log request about byte array in db
</commit_message>
<xml_diff>
--- a/Documentation/GanttChartSprint2.xlsx
+++ b/Documentation/GanttChartSprint2.xlsx
@@ -914,7 +914,7 @@
   <dimension ref="B2:BQ34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1248,10 +1248,14 @@
       <c r="D9" s="16">
         <v>2</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>2</v>
+      </c>
       <c r="G9" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:69" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1264,10 +1268,14 @@
       <c r="D10" s="16">
         <v>3</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
+      <c r="E10" s="16">
+        <v>3</v>
+      </c>
+      <c r="F10" s="16">
+        <v>3</v>
+      </c>
       <c r="G10" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1296,10 +1304,14 @@
       <c r="D12" s="16">
         <v>8</v>
       </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
+      <c r="E12" s="16">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16">
+        <v>5</v>
+      </c>
       <c r="G12" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1312,10 +1324,12 @@
       <c r="D13" s="16">
         <v>3</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="16">
+        <v>6</v>
+      </c>
       <c r="F13" s="16"/>
       <c r="G13" s="17">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="2:69" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>